<commit_message>
Changed name of the PV in SQ15 from *P_SP_TT680 to *P_TT686_min.
</commit_message>
<xml_diff>
--- a/doc/EPICS_dialog_VerticalCryostat_V14.xlsx
+++ b/doc/EPICS_dialog_VerticalCryostat_V14.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13230" windowHeight="6615" tabRatio="595" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13230" windowHeight="6615" tabRatio="595" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,9 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Maxime GUIGNERY - Affichage personnalisé" guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1050" tabRatio="595" activeSheetId="4"/>
+    <customWorkbookView name="Adrien JOURNIAT - Affichage personnalisé" guid="{0FB11559-FF5E-4B68-9C91-951C6118F018}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="855" tabRatio="595" activeSheetId="3"/>
     <customWorkbookView name="Konrad Gajewski - Personal View" guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" mergeInterval="0" personalView="1" xWindow="460" yWindow="46" windowWidth="2045" windowHeight="778" tabRatio="595" activeSheetId="4"/>
-    <customWorkbookView name="Adrien JOURNIAT - Affichage personnalisé" guid="{0FB11559-FF5E-4B68-9C91-951C6118F018}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="855" tabRatio="595" activeSheetId="3"/>
-    <customWorkbookView name="Maxime GUIGNERY - Affichage personnalisé" guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1050" tabRatio="595" activeSheetId="4"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -285,6 +285,40 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Konrad Gajewski</author>
+  </authors>
+  <commentList>
+    <comment ref="P5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Konrad Gajewski:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Changed from SP_TT680</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2936" uniqueCount="1031">
   <si>
@@ -3394,9 +3428,6 @@
     <t>SQ15 : Additional parameters</t>
   </si>
   <si>
-    <t>P_SP_TT680</t>
-  </si>
-  <si>
     <t>P_SP_LT683</t>
   </si>
   <si>
@@ -3842,13 +3873,16 @@
   </si>
   <si>
     <t>Total flow from magnet insert at 2K</t>
+  </si>
+  <si>
+    <t>P_TT686_min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3954,6 +3988,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="21">
@@ -4439,15 +4486,29 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -4479,35 +4540,27 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -4519,15 +4572,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -4543,8 +4592,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -4893,36 +4940,36 @@
         <v>43031</v>
       </c>
       <c r="F2" s="71" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B3" s="39"/>
       <c r="D3" s="28">
         <v>43054</v>
       </c>
       <c r="F3" s="71" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B4" s="40"/>
       <c r="D4" s="28">
         <v>43066</v>
       </c>
       <c r="F4" s="71" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B5" s="41"/>
       <c r="D5" s="28">
@@ -4931,31 +4978,31 @@
     </row>
     <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B6" s="46"/>
       <c r="D6" s="28">
         <v>43082</v>
       </c>
       <c r="F6" s="71" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B7" s="53"/>
       <c r="D7" s="54">
         <v>43160</v>
       </c>
       <c r="F7" s="71" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B8" s="62"/>
       <c r="D8" s="28">
@@ -4964,93 +5011,93 @@
     </row>
     <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B9" s="63"/>
       <c r="D9" s="28">
         <v>44118</v>
       </c>
       <c r="F9" s="71" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="10" spans="1:6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B10" s="65"/>
       <c r="D10" s="28">
         <v>44167</v>
       </c>
       <c r="F10" s="71" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B11" s="68"/>
       <c r="D11" s="28">
         <v>44287</v>
       </c>
       <c r="F11" s="71" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="12" spans="1:6" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D12" s="28">
         <v>44463</v>
       </c>
       <c r="F12" s="71" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B13" s="70"/>
       <c r="D13" s="28">
         <v>44498</v>
       </c>
       <c r="F13" s="71" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B14" s="75"/>
       <c r="D14" s="28">
         <v>44531</v>
       </c>
       <c r="F14" s="71" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="105"/>
+      <c r="B15" s="79"/>
       <c r="D15" s="28">
         <v>44679</v>
       </c>
       <c r="F15" s="71" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}">
-      <selection activeCell="C4" sqref="C4"/>
+    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}">
+      <selection activeCell="D6" sqref="D6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}">
-      <selection activeCell="D6" sqref="D6"/>
+    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}">
+      <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -5118,75 +5165,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
     </row>
     <row r="2" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
     </row>
     <row r="3" spans="2:46" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:46" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="91"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="83"/>
       <c r="K4" s="2" t="s">
         <v>40</v>
       </c>
       <c r="AT4" s="3"/>
     </row>
     <row r="5" spans="2:46" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="82" t="s">
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="89"/>
       <c r="M5" s="1" t="s">
         <v>116</v>
       </c>
       <c r="AT5" s="3"/>
     </row>
     <row r="6" spans="2:46" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="85" t="s">
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="87"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="92"/>
       <c r="K6" s="2" t="s">
         <v>114</v>
       </c>
@@ -5382,50 +5429,50 @@
     </row>
     <row r="18" spans="2:14" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="2:14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="90"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="91"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="83"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="2:14" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B20" s="82" t="s">
+      <c r="B20" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="83" t="s">
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="83"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="84"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="89"/>
       <c r="M20" s="4" t="s">
         <v>321</v>
       </c>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="2:14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="85" t="s">
+      <c r="B21" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="86" t="s">
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="92"/>
+      <c r="F21" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
-      <c r="I21" s="87"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="92"/>
     </row>
     <row r="22" spans="2:14" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
@@ -5586,16 +5633,16 @@
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="2:14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="89" t="s">
+      <c r="B31" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="90"/>
-      <c r="G31" s="90"/>
-      <c r="H31" s="90"/>
-      <c r="I31" s="91"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="83"/>
       <c r="K31" s="2" t="s">
         <v>41</v>
       </c>
@@ -5603,36 +5650,36 @@
       <c r="N31" s="4"/>
     </row>
     <row r="32" spans="2:14" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B32" s="82" t="s">
+      <c r="B32" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="83"/>
-      <c r="D32" s="83"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="82" t="s">
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="83"/>
-      <c r="H32" s="83"/>
-      <c r="I32" s="84"/>
+      <c r="G32" s="88"/>
+      <c r="H32" s="88"/>
+      <c r="I32" s="89"/>
       <c r="M32" s="4" t="s">
         <v>45</v>
       </c>
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="2:29" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="85" t="s">
+      <c r="B33" s="90" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="85" t="s">
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="92"/>
+      <c r="F33" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="G33" s="86"/>
-      <c r="H33" s="86"/>
-      <c r="I33" s="87"/>
+      <c r="G33" s="91"/>
+      <c r="H33" s="91"/>
+      <c r="I33" s="92"/>
       <c r="K33" s="2" t="s">
         <v>42</v>
       </c>
@@ -5866,7 +5913,7 @@
         <v>371</v>
       </c>
       <c r="I42" s="38" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="43" spans="2:29" ht="14.45" x14ac:dyDescent="0.35">
@@ -5881,10 +5928,10 @@
         <v>37</v>
       </c>
       <c r="H43" s="38" t="s">
+        <v>906</v>
+      </c>
+      <c r="I43" s="38" t="s">
         <v>907</v>
-      </c>
-      <c r="I43" s="38" t="s">
-        <v>908</v>
       </c>
       <c r="P43" s="26"/>
       <c r="Q43" s="26"/>
@@ -5947,16 +5994,16 @@
     </row>
     <row r="47" spans="2:29" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="48" spans="2:29" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="89" t="s">
+      <c r="B48" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="90"/>
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="90"/>
-      <c r="H48" s="90"/>
-      <c r="I48" s="91"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="82"/>
+      <c r="E48" s="82"/>
+      <c r="F48" s="82"/>
+      <c r="G48" s="82"/>
+      <c r="H48" s="82"/>
+      <c r="I48" s="83"/>
       <c r="K48" s="2" t="s">
         <v>41</v>
       </c>
@@ -5964,36 +6011,36 @@
       <c r="N48" s="4"/>
     </row>
     <row r="49" spans="2:14" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B49" s="82" t="s">
+      <c r="B49" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="83"/>
-      <c r="D49" s="83"/>
-      <c r="E49" s="84"/>
-      <c r="F49" s="82" t="s">
+      <c r="C49" s="88"/>
+      <c r="D49" s="88"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="G49" s="83"/>
-      <c r="H49" s="83"/>
-      <c r="I49" s="84"/>
+      <c r="G49" s="88"/>
+      <c r="H49" s="88"/>
+      <c r="I49" s="89"/>
       <c r="M49" s="4" t="s">
         <v>45</v>
       </c>
       <c r="N49" s="4"/>
     </row>
     <row r="50" spans="2:14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="85" t="s">
+      <c r="B50" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="86"/>
-      <c r="D50" s="86"/>
-      <c r="E50" s="87"/>
-      <c r="F50" s="85" t="s">
+      <c r="C50" s="91"/>
+      <c r="D50" s="91"/>
+      <c r="E50" s="92"/>
+      <c r="F50" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="G50" s="86"/>
-      <c r="H50" s="86"/>
-      <c r="I50" s="87"/>
+      <c r="G50" s="91"/>
+      <c r="H50" s="91"/>
+      <c r="I50" s="92"/>
       <c r="K50" s="2" t="s">
         <v>42</v>
       </c>
@@ -6074,10 +6121,10 @@
         <v>37</v>
       </c>
       <c r="H53" s="38" t="s">
+        <v>906</v>
+      </c>
+      <c r="I53" s="38" t="s">
         <v>907</v>
-      </c>
-      <c r="I53" s="38" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="54" spans="2:14" ht="14.45" x14ac:dyDescent="0.35">
@@ -6215,16 +6262,16 @@
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="2:14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="89" t="s">
+      <c r="B63" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="90"/>
-      <c r="D63" s="90"/>
-      <c r="E63" s="90"/>
-      <c r="F63" s="90"/>
-      <c r="G63" s="90"/>
-      <c r="H63" s="90"/>
-      <c r="I63" s="91"/>
+      <c r="C63" s="82"/>
+      <c r="D63" s="82"/>
+      <c r="E63" s="82"/>
+      <c r="F63" s="82"/>
+      <c r="G63" s="82"/>
+      <c r="H63" s="82"/>
+      <c r="I63" s="83"/>
       <c r="K63" s="2" t="s">
         <v>41</v>
       </c>
@@ -6232,36 +6279,36 @@
       <c r="N63" s="4"/>
     </row>
     <row r="64" spans="2:14" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B64" s="82" t="s">
+      <c r="B64" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C64" s="83"/>
-      <c r="D64" s="83"/>
-      <c r="E64" s="84"/>
-      <c r="F64" s="83" t="s">
+      <c r="C64" s="88"/>
+      <c r="D64" s="88"/>
+      <c r="E64" s="89"/>
+      <c r="F64" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="G64" s="83"/>
-      <c r="H64" s="83"/>
-      <c r="I64" s="84"/>
+      <c r="G64" s="88"/>
+      <c r="H64" s="88"/>
+      <c r="I64" s="89"/>
       <c r="M64" s="4" t="s">
         <v>48</v>
       </c>
       <c r="N64" s="4"/>
     </row>
     <row r="65" spans="2:46" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="79" t="s">
+      <c r="B65" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="C65" s="80"/>
-      <c r="D65" s="80"/>
-      <c r="E65" s="81"/>
-      <c r="F65" s="80" t="s">
+      <c r="C65" s="95"/>
+      <c r="D65" s="95"/>
+      <c r="E65" s="96"/>
+      <c r="F65" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="G65" s="80"/>
-      <c r="H65" s="80"/>
-      <c r="I65" s="81"/>
+      <c r="G65" s="95"/>
+      <c r="H65" s="95"/>
+      <c r="I65" s="96"/>
       <c r="K65" s="2" t="s">
         <v>42</v>
       </c>
@@ -6426,16 +6473,16 @@
       <c r="AT74" s="3"/>
     </row>
     <row r="75" spans="2:46" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B75" s="89" t="s">
+      <c r="B75" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="C75" s="90"/>
-      <c r="D75" s="90"/>
-      <c r="E75" s="90"/>
-      <c r="F75" s="90"/>
-      <c r="G75" s="90"/>
-      <c r="H75" s="90"/>
-      <c r="I75" s="91"/>
+      <c r="C75" s="82"/>
+      <c r="D75" s="82"/>
+      <c r="E75" s="82"/>
+      <c r="F75" s="82"/>
+      <c r="G75" s="82"/>
+      <c r="H75" s="82"/>
+      <c r="I75" s="83"/>
       <c r="K75" s="2" t="s">
         <v>145</v>
       </c>
@@ -6444,36 +6491,36 @@
       <c r="AT75" s="3"/>
     </row>
     <row r="76" spans="2:46" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B76" s="82" t="s">
+      <c r="B76" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="83"/>
-      <c r="D76" s="83"/>
-      <c r="E76" s="84"/>
-      <c r="F76" s="83" t="s">
+      <c r="C76" s="88"/>
+      <c r="D76" s="88"/>
+      <c r="E76" s="89"/>
+      <c r="F76" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="G76" s="83"/>
-      <c r="H76" s="83"/>
-      <c r="I76" s="84"/>
+      <c r="G76" s="88"/>
+      <c r="H76" s="88"/>
+      <c r="I76" s="89"/>
       <c r="M76" s="1" t="s">
         <v>50</v>
       </c>
       <c r="AT76" s="3"/>
     </row>
     <row r="77" spans="2:46" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B77" s="85" t="s">
+      <c r="B77" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="C77" s="86"/>
-      <c r="D77" s="86"/>
-      <c r="E77" s="87"/>
-      <c r="F77" s="86" t="s">
+      <c r="C77" s="91"/>
+      <c r="D77" s="91"/>
+      <c r="E77" s="92"/>
+      <c r="F77" s="91" t="s">
         <v>69</v>
       </c>
-      <c r="G77" s="86"/>
-      <c r="H77" s="86"/>
-      <c r="I77" s="87"/>
+      <c r="G77" s="91"/>
+      <c r="H77" s="91"/>
+      <c r="I77" s="92"/>
       <c r="M77" s="4" t="s">
         <v>51</v>
       </c>
@@ -6560,10 +6607,10 @@
         <v>37</v>
       </c>
       <c r="H80" s="72" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I80" s="73" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="M80" s="2" t="s">
         <v>146</v>
@@ -6591,10 +6638,10 @@
         <v>37</v>
       </c>
       <c r="H81" s="72" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I81" s="73" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="O81" s="4" t="s">
         <v>55</v>
@@ -6621,10 +6668,10 @@
         <v>37</v>
       </c>
       <c r="H82" s="72" t="s">
+        <v>1006</v>
+      </c>
+      <c r="I82" s="73" t="s">
         <v>1007</v>
-      </c>
-      <c r="I82" s="73" t="s">
-        <v>1008</v>
       </c>
       <c r="M82" s="2" t="s">
         <v>147</v>
@@ -6658,10 +6705,10 @@
         <v>37</v>
       </c>
       <c r="D84" s="72" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="E84" s="73" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
@@ -6692,10 +6739,10 @@
         <v>37</v>
       </c>
       <c r="D85" s="72" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="E85" s="73" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>25</v>
@@ -6866,19 +6913,19 @@
       <c r="AT92" s="3"/>
     </row>
     <row r="93" spans="2:46" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="89" t="s">
-        <v>983</v>
-      </c>
-      <c r="C93" s="90"/>
-      <c r="D93" s="90"/>
-      <c r="E93" s="90"/>
-      <c r="F93" s="90"/>
-      <c r="G93" s="90"/>
-      <c r="H93" s="90"/>
-      <c r="I93" s="91"/>
+      <c r="B93" s="81" t="s">
+        <v>982</v>
+      </c>
+      <c r="C93" s="82"/>
+      <c r="D93" s="82"/>
+      <c r="E93" s="82"/>
+      <c r="F93" s="82"/>
+      <c r="G93" s="82"/>
+      <c r="H93" s="82"/>
+      <c r="I93" s="83"/>
       <c r="L93" s="69"/>
       <c r="M93" s="69" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="N93" s="4"/>
       <c r="P93" s="26"/>
@@ -6898,18 +6945,18 @@
       <c r="AT93" s="3"/>
     </row>
     <row r="94" spans="2:46" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="82" t="s">
+      <c r="B94" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C94" s="83"/>
-      <c r="D94" s="83"/>
-      <c r="E94" s="84"/>
-      <c r="F94" s="83" t="s">
+      <c r="C94" s="88"/>
+      <c r="D94" s="88"/>
+      <c r="E94" s="89"/>
+      <c r="F94" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="G94" s="83"/>
-      <c r="H94" s="83"/>
-      <c r="I94" s="84"/>
+      <c r="G94" s="88"/>
+      <c r="H94" s="88"/>
+      <c r="I94" s="89"/>
       <c r="L94" s="69"/>
       <c r="M94" s="69"/>
       <c r="P94" s="26"/>
@@ -6929,18 +6976,18 @@
       <c r="AT94" s="3"/>
     </row>
     <row r="95" spans="2:46" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="85" t="s">
-        <v>984</v>
-      </c>
-      <c r="C95" s="86"/>
-      <c r="D95" s="86"/>
-      <c r="E95" s="87"/>
-      <c r="F95" s="86" t="s">
-        <v>986</v>
-      </c>
-      <c r="G95" s="86"/>
-      <c r="H95" s="86"/>
-      <c r="I95" s="87"/>
+      <c r="B95" s="90" t="s">
+        <v>983</v>
+      </c>
+      <c r="C95" s="91"/>
+      <c r="D95" s="91"/>
+      <c r="E95" s="92"/>
+      <c r="F95" s="91" t="s">
+        <v>985</v>
+      </c>
+      <c r="G95" s="91"/>
+      <c r="H95" s="91"/>
+      <c r="I95" s="92"/>
       <c r="L95" s="69"/>
       <c r="M95" s="69"/>
       <c r="N95" s="4"/>
@@ -6971,7 +7018,7 @@
         <v>117</v>
       </c>
       <c r="E96" s="15" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
@@ -7006,7 +7053,7 @@
         <v>82</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
@@ -7041,7 +7088,7 @@
         <v>138</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="4"/>
@@ -7077,7 +7124,7 @@
         <v>140</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="4"/>
@@ -7113,7 +7160,7 @@
         <v>326</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="4"/>
@@ -7149,7 +7196,7 @@
         <v>328</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
@@ -7185,7 +7232,7 @@
         <v>328</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
@@ -7220,7 +7267,7 @@
         <v>328</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
@@ -7255,7 +7302,7 @@
         <v>328</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
@@ -7290,7 +7337,7 @@
         <v>328</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
@@ -7325,7 +7372,7 @@
         <v>328</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
@@ -7357,10 +7404,10 @@
         <v>37</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
@@ -7392,10 +7439,10 @@
         <v>37</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
@@ -7427,10 +7474,10 @@
         <v>37</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
@@ -7489,7 +7536,7 @@
         <v>38</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E111" s="7" t="s">
         <v>78</v>
@@ -7524,10 +7571,10 @@
         <v>38</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="E112" s="7" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
@@ -7559,10 +7606,10 @@
         <v>38</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
@@ -7716,16 +7763,16 @@
       <c r="AT118" s="3"/>
     </row>
     <row r="119" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="92" t="s">
+      <c r="B119" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="C119" s="93"/>
-      <c r="D119" s="93"/>
-      <c r="E119" s="93"/>
-      <c r="F119" s="93"/>
-      <c r="G119" s="93"/>
-      <c r="H119" s="93"/>
-      <c r="I119" s="94"/>
+      <c r="C119" s="85"/>
+      <c r="D119" s="85"/>
+      <c r="E119" s="85"/>
+      <c r="F119" s="85"/>
+      <c r="G119" s="85"/>
+      <c r="H119" s="85"/>
+      <c r="I119" s="86"/>
       <c r="K119" s="2" t="s">
         <v>41</v>
       </c>
@@ -7748,18 +7795,18 @@
       <c r="AT119" s="3"/>
     </row>
     <row r="120" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B120" s="82" t="s">
+      <c r="B120" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C120" s="83"/>
-      <c r="D120" s="83"/>
-      <c r="E120" s="84"/>
-      <c r="F120" s="82" t="s">
+      <c r="C120" s="88"/>
+      <c r="D120" s="88"/>
+      <c r="E120" s="89"/>
+      <c r="F120" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="G120" s="83"/>
-      <c r="H120" s="83"/>
-      <c r="I120" s="84"/>
+      <c r="G120" s="88"/>
+      <c r="H120" s="88"/>
+      <c r="I120" s="89"/>
       <c r="M120" s="4" t="s">
         <v>45</v>
       </c>
@@ -7781,18 +7828,18 @@
       <c r="AT120" s="3"/>
     </row>
     <row r="121" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="85" t="s">
+      <c r="B121" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="C121" s="86"/>
-      <c r="D121" s="86"/>
-      <c r="E121" s="87"/>
-      <c r="F121" s="85" t="s">
+      <c r="C121" s="91"/>
+      <c r="D121" s="91"/>
+      <c r="E121" s="92"/>
+      <c r="F121" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="G121" s="86"/>
-      <c r="H121" s="86"/>
-      <c r="I121" s="87"/>
+      <c r="G121" s="91"/>
+      <c r="H121" s="91"/>
+      <c r="I121" s="92"/>
       <c r="K121" s="2" t="s">
         <v>42</v>
       </c>
@@ -7946,10 +7993,10 @@
         <v>37</v>
       </c>
       <c r="H125" s="38" t="s">
+        <v>906</v>
+      </c>
+      <c r="I125" s="38" t="s">
         <v>907</v>
-      </c>
-      <c r="I125" s="38" t="s">
-        <v>908</v>
       </c>
       <c r="M125" s="1" t="s">
         <v>80</v>
@@ -7978,7 +8025,7 @@
         <v>346</v>
       </c>
       <c r="I126" s="38" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="127" spans="2:46" x14ac:dyDescent="0.25">
@@ -8192,16 +8239,16 @@
       <c r="I141" s="4"/>
     </row>
     <row r="142" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="89" t="s">
+      <c r="B142" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="C142" s="90"/>
-      <c r="D142" s="90"/>
-      <c r="E142" s="90"/>
-      <c r="F142" s="90"/>
-      <c r="G142" s="90"/>
-      <c r="H142" s="90"/>
-      <c r="I142" s="91"/>
+      <c r="C142" s="82"/>
+      <c r="D142" s="82"/>
+      <c r="E142" s="82"/>
+      <c r="F142" s="82"/>
+      <c r="G142" s="82"/>
+      <c r="H142" s="82"/>
+      <c r="I142" s="83"/>
       <c r="K142" s="2" t="s">
         <v>41</v>
       </c>
@@ -8209,36 +8256,36 @@
       <c r="N142" s="4"/>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B143" s="82" t="s">
+      <c r="B143" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C143" s="83"/>
-      <c r="D143" s="83"/>
-      <c r="E143" s="84"/>
-      <c r="F143" s="83" t="s">
+      <c r="C143" s="88"/>
+      <c r="D143" s="88"/>
+      <c r="E143" s="89"/>
+      <c r="F143" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="G143" s="83"/>
-      <c r="H143" s="83"/>
-      <c r="I143" s="84"/>
+      <c r="G143" s="88"/>
+      <c r="H143" s="88"/>
+      <c r="I143" s="89"/>
       <c r="M143" s="4" t="s">
         <v>59</v>
       </c>
       <c r="N143" s="4"/>
     </row>
     <row r="144" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="79" t="s">
+      <c r="B144" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="C144" s="80"/>
-      <c r="D144" s="80"/>
-      <c r="E144" s="81"/>
-      <c r="F144" s="80" t="s">
+      <c r="C144" s="95"/>
+      <c r="D144" s="95"/>
+      <c r="E144" s="96"/>
+      <c r="F144" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="G144" s="80"/>
-      <c r="H144" s="80"/>
-      <c r="I144" s="81"/>
+      <c r="G144" s="95"/>
+      <c r="H144" s="95"/>
+      <c r="I144" s="96"/>
       <c r="K144" s="2" t="s">
         <v>42</v>
       </c>
@@ -8695,9 +8742,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" topLeftCell="A106">
+    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}" scale="70">
       <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G104" sqref="G104"/>
+      <selection pane="topRight" activeCell="F69" sqref="F69:I69"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
     </customSheetView>
@@ -8707,28 +8754,30 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}" scale="70">
+    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" topLeftCell="A106">
       <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F69" sqref="F69:I69"/>
+      <selection pane="topRight" activeCell="G104" sqref="G104"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="46">
-    <mergeCell ref="B75:I75"/>
-    <mergeCell ref="B119:I119"/>
-    <mergeCell ref="B142:I142"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="F76:I76"/>
-    <mergeCell ref="B120:E120"/>
-    <mergeCell ref="F120:I120"/>
-    <mergeCell ref="B121:E121"/>
-    <mergeCell ref="F121:I121"/>
-    <mergeCell ref="B93:I93"/>
-    <mergeCell ref="B94:E94"/>
-    <mergeCell ref="F94:I94"/>
-    <mergeCell ref="B95:E95"/>
-    <mergeCell ref="F95:I95"/>
+    <mergeCell ref="B144:E144"/>
+    <mergeCell ref="F144:I144"/>
+    <mergeCell ref="B143:E143"/>
+    <mergeCell ref="F143:I143"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="F77:I77"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="B64:E64"/>
@@ -8745,22 +8794,20 @@
     <mergeCell ref="B49:E49"/>
     <mergeCell ref="F49:I49"/>
     <mergeCell ref="B63:I63"/>
-    <mergeCell ref="B144:E144"/>
-    <mergeCell ref="F144:I144"/>
-    <mergeCell ref="B143:E143"/>
-    <mergeCell ref="F143:I143"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="B33:E33"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="F65:I65"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="F77:I77"/>
+    <mergeCell ref="B75:I75"/>
+    <mergeCell ref="B119:I119"/>
+    <mergeCell ref="B142:I142"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="F76:I76"/>
+    <mergeCell ref="B120:E120"/>
+    <mergeCell ref="F120:I120"/>
+    <mergeCell ref="B121:E121"/>
+    <mergeCell ref="F121:I121"/>
+    <mergeCell ref="B93:I93"/>
+    <mergeCell ref="B94:E94"/>
+    <mergeCell ref="F94:I94"/>
+    <mergeCell ref="B95:E95"/>
+    <mergeCell ref="F95:I95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
@@ -8775,7 +8822,7 @@
   <dimension ref="A1:BH124"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="AI35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="AZ35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="O42" sqref="O42"/>
@@ -8904,355 +8951,355 @@
       <c r="BH1" s="2"/>
     </row>
     <row r="2" spans="1:60" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="84" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
       <c r="F2" s="20"/>
-      <c r="G2" s="97" t="s">
+      <c r="G2" s="100" t="s">
         <v>274</v>
       </c>
-      <c r="H2" s="98"/>
-      <c r="I2" s="97" t="s">
+      <c r="H2" s="101"/>
+      <c r="I2" s="100" t="s">
         <v>559</v>
       </c>
-      <c r="J2" s="98"/>
-      <c r="K2" s="97" t="s">
+      <c r="J2" s="101"/>
+      <c r="K2" s="100" t="s">
         <v>560</v>
       </c>
-      <c r="L2" s="98"/>
-      <c r="M2" s="97" t="s">
+      <c r="L2" s="101"/>
+      <c r="M2" s="100" t="s">
         <v>561</v>
       </c>
-      <c r="N2" s="98"/>
-      <c r="O2" s="97" t="s">
+      <c r="N2" s="101"/>
+      <c r="O2" s="100" t="s">
         <v>562</v>
       </c>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="97" t="s">
+      <c r="P2" s="101"/>
+      <c r="Q2" s="100" t="s">
         <v>563</v>
       </c>
-      <c r="R2" s="98"/>
-      <c r="S2" s="97" t="s">
+      <c r="R2" s="101"/>
+      <c r="S2" s="100" t="s">
         <v>564</v>
       </c>
-      <c r="T2" s="98"/>
-      <c r="U2" s="97" t="s">
+      <c r="T2" s="101"/>
+      <c r="U2" s="100" t="s">
         <v>565</v>
       </c>
-      <c r="V2" s="98"/>
-      <c r="W2" s="97" t="s">
+      <c r="V2" s="101"/>
+      <c r="W2" s="100" t="s">
         <v>566</v>
       </c>
-      <c r="X2" s="98"/>
-      <c r="Y2" s="97" t="s">
+      <c r="X2" s="101"/>
+      <c r="Y2" s="100" t="s">
         <v>567</v>
       </c>
-      <c r="Z2" s="98"/>
-      <c r="AA2" s="97" t="s">
+      <c r="Z2" s="101"/>
+      <c r="AA2" s="100" t="s">
         <v>568</v>
       </c>
-      <c r="AB2" s="98"/>
-      <c r="AC2" s="97" t="s">
+      <c r="AB2" s="101"/>
+      <c r="AC2" s="100" t="s">
         <v>569</v>
       </c>
-      <c r="AD2" s="98"/>
-      <c r="AE2" s="97" t="s">
+      <c r="AD2" s="101"/>
+      <c r="AE2" s="100" t="s">
         <v>570</v>
       </c>
-      <c r="AF2" s="98"/>
-      <c r="AG2" s="97" t="s">
+      <c r="AF2" s="101"/>
+      <c r="AG2" s="100" t="s">
         <v>571</v>
       </c>
-      <c r="AH2" s="98"/>
-      <c r="AI2" s="97" t="s">
-        <v>962</v>
-      </c>
-      <c r="AJ2" s="98"/>
-      <c r="AK2" s="97" t="s">
+      <c r="AH2" s="101"/>
+      <c r="AI2" s="100" t="s">
+        <v>961</v>
+      </c>
+      <c r="AJ2" s="101"/>
+      <c r="AK2" s="100" t="s">
         <v>572</v>
       </c>
-      <c r="AL2" s="98"/>
-      <c r="AM2" s="97" t="s">
+      <c r="AL2" s="101"/>
+      <c r="AM2" s="100" t="s">
         <v>573</v>
       </c>
-      <c r="AN2" s="98"/>
-      <c r="AO2" s="97" t="s">
+      <c r="AN2" s="101"/>
+      <c r="AO2" s="100" t="s">
         <v>574</v>
       </c>
-      <c r="AP2" s="98"/>
-      <c r="AQ2" s="97" t="s">
+      <c r="AP2" s="101"/>
+      <c r="AQ2" s="100" t="s">
         <v>575</v>
       </c>
-      <c r="AR2" s="98"/>
-      <c r="AS2" s="97" t="s">
+      <c r="AR2" s="101"/>
+      <c r="AS2" s="100" t="s">
         <v>576</v>
       </c>
-      <c r="AT2" s="98"/>
-      <c r="AU2" s="97" t="s">
+      <c r="AT2" s="101"/>
+      <c r="AU2" s="100" t="s">
         <v>577</v>
       </c>
-      <c r="AV2" s="98"/>
-      <c r="AW2" s="97" t="s">
+      <c r="AV2" s="101"/>
+      <c r="AW2" s="100" t="s">
         <v>578</v>
       </c>
-      <c r="AX2" s="98"/>
-      <c r="AY2" s="97" t="s">
+      <c r="AX2" s="101"/>
+      <c r="AY2" s="100" t="s">
         <v>579</v>
       </c>
-      <c r="AZ2" s="98"/>
-      <c r="BA2" s="97" t="s">
+      <c r="AZ2" s="101"/>
+      <c r="BA2" s="100" t="s">
         <v>580</v>
       </c>
-      <c r="BB2" s="98"/>
-      <c r="BC2" s="97" t="s">
+      <c r="BB2" s="101"/>
+      <c r="BC2" s="100" t="s">
         <v>581</v>
       </c>
-      <c r="BD2" s="98"/>
-      <c r="BE2" s="97" t="s">
+      <c r="BD2" s="101"/>
+      <c r="BE2" s="100" t="s">
         <v>582</v>
       </c>
-      <c r="BF2" s="98"/>
-      <c r="BG2" s="97" t="s">
+      <c r="BF2" s="101"/>
+      <c r="BG2" s="100" t="s">
         <v>583</v>
       </c>
-      <c r="BH2" s="98"/>
+      <c r="BH2" s="101"/>
     </row>
     <row r="3" spans="1:60" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="106"/>
       <c r="F3" s="20"/>
-      <c r="G3" s="82" t="s">
+      <c r="G3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="I3" s="82" t="s">
+      <c r="I3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="J3" s="84" t="s">
+      <c r="J3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="K3" s="82" t="s">
+      <c r="K3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="L3" s="84" t="s">
+      <c r="L3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="M3" s="82" t="s">
+      <c r="M3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="N3" s="84" t="s">
+      <c r="N3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="O3" s="82" t="s">
+      <c r="O3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="P3" s="84" t="s">
+      <c r="P3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="Q3" s="82" t="s">
+      <c r="Q3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="R3" s="84" t="s">
+      <c r="R3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="S3" s="82" t="s">
+      <c r="S3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="T3" s="84" t="s">
+      <c r="T3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="U3" s="82" t="s">
+      <c r="U3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="V3" s="84" t="s">
+      <c r="V3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="W3" s="82" t="s">
+      <c r="W3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="X3" s="84" t="s">
+      <c r="X3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="Y3" s="82" t="s">
+      <c r="Y3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="Z3" s="84" t="s">
+      <c r="Z3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AA3" s="82" t="s">
+      <c r="AA3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AB3" s="84" t="s">
+      <c r="AB3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AC3" s="82" t="s">
+      <c r="AC3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AD3" s="84" t="s">
+      <c r="AD3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AE3" s="82" t="s">
+      <c r="AE3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AF3" s="84" t="s">
+      <c r="AF3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AG3" s="82" t="s">
+      <c r="AG3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AH3" s="84" t="s">
+      <c r="AH3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AI3" s="82" t="s">
+      <c r="AI3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AJ3" s="84" t="s">
+      <c r="AJ3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AK3" s="82" t="s">
+      <c r="AK3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AL3" s="84" t="s">
+      <c r="AL3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AM3" s="82" t="s">
+      <c r="AM3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AN3" s="84" t="s">
+      <c r="AN3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AO3" s="82" t="s">
+      <c r="AO3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AP3" s="84" t="s">
+      <c r="AP3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AQ3" s="82" t="s">
+      <c r="AQ3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AR3" s="84" t="s">
+      <c r="AR3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AS3" s="82" t="s">
+      <c r="AS3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AT3" s="84" t="s">
+      <c r="AT3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AU3" s="82" t="s">
+      <c r="AU3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AV3" s="84" t="s">
+      <c r="AV3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AW3" s="82" t="s">
+      <c r="AW3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AX3" s="84" t="s">
+      <c r="AX3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="AY3" s="82" t="s">
+      <c r="AY3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="AZ3" s="84" t="s">
+      <c r="AZ3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="BA3" s="82" t="s">
+      <c r="BA3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="BB3" s="84" t="s">
+      <c r="BB3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="BC3" s="82" t="s">
+      <c r="BC3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="BD3" s="84" t="s">
+      <c r="BD3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="BE3" s="82" t="s">
+      <c r="BE3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="BF3" s="84" t="s">
+      <c r="BF3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="BG3" s="82" t="s">
+      <c r="BG3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="BH3" s="84" t="s">
+      <c r="BH3" s="89" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:60" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="97" t="s">
         <v>156</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99"/>
       <c r="F4" s="21"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="96"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="95"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="95"/>
-      <c r="U4" s="96"/>
-      <c r="V4" s="95"/>
-      <c r="W4" s="96"/>
-      <c r="X4" s="95"/>
-      <c r="Y4" s="96"/>
-      <c r="Z4" s="95"/>
-      <c r="AA4" s="96"/>
-      <c r="AB4" s="95"/>
-      <c r="AC4" s="96"/>
-      <c r="AD4" s="95"/>
-      <c r="AE4" s="96"/>
-      <c r="AF4" s="95"/>
-      <c r="AG4" s="96"/>
-      <c r="AH4" s="95"/>
-      <c r="AI4" s="96"/>
-      <c r="AJ4" s="95"/>
-      <c r="AK4" s="96"/>
-      <c r="AL4" s="95"/>
-      <c r="AM4" s="96"/>
-      <c r="AN4" s="95"/>
-      <c r="AO4" s="96"/>
-      <c r="AP4" s="95"/>
-      <c r="AQ4" s="96"/>
-      <c r="AR4" s="95"/>
-      <c r="AS4" s="96"/>
-      <c r="AT4" s="95"/>
-      <c r="AU4" s="96"/>
-      <c r="AV4" s="95"/>
-      <c r="AW4" s="96"/>
-      <c r="AX4" s="95"/>
-      <c r="AY4" s="96"/>
-      <c r="AZ4" s="95"/>
-      <c r="BA4" s="96"/>
-      <c r="BB4" s="95"/>
-      <c r="BC4" s="96"/>
-      <c r="BD4" s="95"/>
-      <c r="BE4" s="96"/>
-      <c r="BF4" s="95"/>
-      <c r="BG4" s="96"/>
-      <c r="BH4" s="95"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="102"/>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="103"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="103"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="103"/>
+      <c r="W4" s="102"/>
+      <c r="X4" s="103"/>
+      <c r="Y4" s="102"/>
+      <c r="Z4" s="103"/>
+      <c r="AA4" s="102"/>
+      <c r="AB4" s="103"/>
+      <c r="AC4" s="102"/>
+      <c r="AD4" s="103"/>
+      <c r="AE4" s="102"/>
+      <c r="AF4" s="103"/>
+      <c r="AG4" s="102"/>
+      <c r="AH4" s="103"/>
+      <c r="AI4" s="102"/>
+      <c r="AJ4" s="103"/>
+      <c r="AK4" s="102"/>
+      <c r="AL4" s="103"/>
+      <c r="AM4" s="102"/>
+      <c r="AN4" s="103"/>
+      <c r="AO4" s="102"/>
+      <c r="AP4" s="103"/>
+      <c r="AQ4" s="102"/>
+      <c r="AR4" s="103"/>
+      <c r="AS4" s="102"/>
+      <c r="AT4" s="103"/>
+      <c r="AU4" s="102"/>
+      <c r="AV4" s="103"/>
+      <c r="AW4" s="102"/>
+      <c r="AX4" s="103"/>
+      <c r="AY4" s="102"/>
+      <c r="AZ4" s="103"/>
+      <c r="BA4" s="102"/>
+      <c r="BB4" s="103"/>
+      <c r="BC4" s="102"/>
+      <c r="BD4" s="103"/>
+      <c r="BE4" s="102"/>
+      <c r="BF4" s="103"/>
+      <c r="BG4" s="102"/>
+      <c r="BH4" s="103"/>
     </row>
     <row r="5" spans="1:60" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
@@ -10143,10 +10190,10 @@
         <v>37</v>
       </c>
       <c r="D14" s="58" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="16"/>
@@ -10192,10 +10239,10 @@
       <c r="AQ14" s="16"/>
       <c r="AR14" s="16"/>
       <c r="AS14" s="66" t="s">
+        <v>978</v>
+      </c>
+      <c r="AT14" s="66" t="s">
         <v>979</v>
-      </c>
-      <c r="AT14" s="66" t="s">
-        <v>980</v>
       </c>
       <c r="AU14" s="16"/>
       <c r="AV14" s="16"/>
@@ -10220,10 +10267,10 @@
         <v>37</v>
       </c>
       <c r="D15" s="58" t="s">
+        <v>957</v>
+      </c>
+      <c r="E15" s="59" t="s">
         <v>958</v>
-      </c>
-      <c r="E15" s="59" t="s">
-        <v>959</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="16"/>
@@ -10401,10 +10448,10 @@
       <c r="AS17" s="16"/>
       <c r="AT17" s="16"/>
       <c r="AU17" s="16" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="AV17" s="16" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="AW17" s="16"/>
       <c r="AX17" s="16"/>
@@ -10482,10 +10529,10 @@
       <c r="AS18" s="16"/>
       <c r="AT18" s="16"/>
       <c r="AU18" s="16" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="AV18" s="16" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="AW18" s="16"/>
       <c r="AX18" s="16"/>
@@ -10555,10 +10602,10 @@
       <c r="AS19" s="16"/>
       <c r="AT19" s="16"/>
       <c r="AU19" s="16" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="AV19" s="16" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="AW19" s="16"/>
       <c r="AX19" s="16"/>
@@ -10628,10 +10675,10 @@
       <c r="AS20" s="16"/>
       <c r="AT20" s="16"/>
       <c r="AU20" s="16" t="s">
+        <v>891</v>
+      </c>
+      <c r="AV20" s="16" t="s">
         <v>892</v>
-      </c>
-      <c r="AV20" s="16" t="s">
-        <v>893</v>
       </c>
       <c r="AW20" s="16"/>
       <c r="AX20" s="16"/>
@@ -11315,7 +11362,7 @@
       <c r="AS29" s="16"/>
       <c r="AT29" s="16"/>
       <c r="AU29" s="16" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="AV29" s="16" t="s">
         <v>798</v>
@@ -11400,7 +11447,7 @@
       <c r="AS30" s="16"/>
       <c r="AT30" s="16"/>
       <c r="AU30" s="16" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="AV30" s="16" t="s">
         <v>798</v>
@@ -11485,7 +11532,7 @@
       <c r="AS31" s="16"/>
       <c r="AT31" s="16"/>
       <c r="AU31" s="16" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="AV31" s="16" t="s">
         <v>798</v>
@@ -11558,7 +11605,7 @@
       <c r="AS32" s="16"/>
       <c r="AT32" s="16"/>
       <c r="AU32" s="16" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="AV32" s="16" t="s">
         <v>798</v>
@@ -11907,7 +11954,7 @@
         <v>799</v>
       </c>
       <c r="AV36" s="16" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="AW36" s="16" t="s">
         <v>811</v>
@@ -12081,10 +12128,10 @@
         <v>813</v>
       </c>
       <c r="AY37" s="16" t="s">
+        <v>897</v>
+      </c>
+      <c r="AZ37" s="1" t="s">
         <v>898</v>
-      </c>
-      <c r="AZ37" s="1" t="s">
-        <v>899</v>
       </c>
       <c r="BA37" s="16" t="s">
         <v>658</v>
@@ -12105,10 +12152,10 @@
         <v>755</v>
       </c>
       <c r="BG37" s="16" t="s">
+        <v>902</v>
+      </c>
+      <c r="BH37" s="1" t="s">
         <v>903</v>
-      </c>
-      <c r="BH37" s="1" t="s">
-        <v>904</v>
       </c>
     </row>
     <row r="38" spans="2:60" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
@@ -12241,7 +12288,7 @@
         <v>802</v>
       </c>
       <c r="AV38" s="16" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="AW38" s="16" t="s">
         <v>814</v>
@@ -12257,16 +12304,16 @@
         <v>755</v>
       </c>
       <c r="BC38" s="16" t="s">
+        <v>901</v>
+      </c>
+      <c r="BD38" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="BE38" s="16" t="s">
         <v>902</v>
       </c>
-      <c r="BD38" s="1" t="s">
-        <v>899</v>
-      </c>
-      <c r="BE38" s="16" t="s">
+      <c r="BF38" s="16" t="s">
         <v>903</v>
-      </c>
-      <c r="BF38" s="16" t="s">
-        <v>904</v>
       </c>
       <c r="BG38" s="16"/>
       <c r="BH38" s="16"/>
@@ -12411,16 +12458,16 @@
       </c>
       <c r="AY39" s="16"/>
       <c r="BA39" s="16" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="BB39" s="16" t="s">
+        <v>898</v>
+      </c>
+      <c r="BC39" s="16" t="s">
         <v>899</v>
       </c>
-      <c r="BC39" s="16" t="s">
-        <v>900</v>
-      </c>
       <c r="BD39" s="16" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="BE39" s="16"/>
       <c r="BF39" s="16"/>
@@ -12531,7 +12578,7 @@
         <v>775</v>
       </c>
       <c r="AR40" s="16" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="AS40" s="16" t="s">
         <v>793</v>
@@ -12543,7 +12590,7 @@
         <v>805</v>
       </c>
       <c r="AV40" s="16" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="AW40" s="16" t="s">
         <v>873</v>
@@ -12553,16 +12600,16 @@
       </c>
       <c r="AY40" s="16"/>
       <c r="BA40" s="16" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="BB40" s="16" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="BC40" s="16" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="BD40" s="16" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="BE40" s="16"/>
       <c r="BF40" s="16"/>
@@ -12663,10 +12710,10 @@
       </c>
       <c r="AO41" s="16"/>
       <c r="AQ41" s="16" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="AR41" s="16" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="AS41" s="16" t="s">
         <v>658</v>
@@ -12688,16 +12735,16 @@
       </c>
       <c r="AY41" s="16"/>
       <c r="BA41" s="64" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="BB41" s="64" t="s">
+        <v>968</v>
+      </c>
+      <c r="BC41" s="64" t="s">
         <v>969</v>
       </c>
-      <c r="BC41" s="64" t="s">
-        <v>970</v>
-      </c>
       <c r="BD41" s="64" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="BE41" s="16"/>
       <c r="BF41" s="16"/>
@@ -12806,7 +12853,7 @@
         <v>808</v>
       </c>
       <c r="AV42" s="16" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="AW42" s="16" t="s">
         <v>751</v>
@@ -12915,10 +12962,10 @@
       <c r="AQ43" s="16"/>
       <c r="AR43" s="16"/>
       <c r="AS43" s="66" t="s">
+        <v>971</v>
+      </c>
+      <c r="AT43" s="66" t="s">
         <v>972</v>
-      </c>
-      <c r="AT43" s="66" t="s">
-        <v>973</v>
       </c>
       <c r="AU43" s="1" t="s">
         <v>809</v>
@@ -13867,12 +13914,12 @@
       <c r="BH55" s="16"/>
     </row>
     <row r="56" spans="2:60" s="1" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="92" t="s">
+      <c r="B56" s="84" t="s">
         <v>155</v>
       </c>
-      <c r="C56" s="93"/>
-      <c r="D56" s="93"/>
-      <c r="E56" s="94"/>
+      <c r="C56" s="85"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="86"/>
       <c r="F56" s="8"/>
       <c r="G56" s="16"/>
       <c r="H56" s="16"/>
@@ -13930,12 +13977,12 @@
       <c r="BH56" s="16"/>
     </row>
     <row r="57" spans="2:60" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B57" s="102" t="s">
+      <c r="B57" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="103"/>
-      <c r="D57" s="103"/>
-      <c r="E57" s="104"/>
+      <c r="C57" s="105"/>
+      <c r="D57" s="105"/>
+      <c r="E57" s="106"/>
       <c r="F57" s="20"/>
       <c r="G57" s="16"/>
       <c r="H57" s="16"/>
@@ -13993,12 +14040,12 @@
       <c r="BH57" s="16"/>
     </row>
     <row r="58" spans="2:60" s="1" customFormat="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="99" t="s">
+      <c r="B58" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="C58" s="100"/>
-      <c r="D58" s="100"/>
-      <c r="E58" s="101"/>
+      <c r="C58" s="98"/>
+      <c r="D58" s="98"/>
+      <c r="E58" s="99"/>
       <c r="F58" s="21"/>
       <c r="G58" s="16"/>
       <c r="H58" s="16"/>
@@ -14684,10 +14731,10 @@
         <v>37</v>
       </c>
       <c r="D68" s="47" t="s">
+        <v>949</v>
+      </c>
+      <c r="E68" s="49" t="s">
         <v>950</v>
-      </c>
-      <c r="E68" s="49" t="s">
-        <v>951</v>
       </c>
       <c r="F68" s="8"/>
       <c r="G68" s="16"/>
@@ -18952,9 +18999,9 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" scale="60">
-      <pane xSplit="5" ySplit="4" topLeftCell="I14" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H70" sqref="H70"/>
+    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}" scale="70">
+      <pane xSplit="5" ySplit="4" topLeftCell="F62" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="I77" sqref="I77:BF77"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -18964,14 +19011,89 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}" scale="70">
-      <pane xSplit="5" ySplit="4" topLeftCell="F62" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I77" sqref="I77:BF77"/>
+    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" scale="60">
+      <pane xSplit="5" ySplit="4" topLeftCell="I14" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H70" sqref="H70"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="87">
+    <mergeCell ref="BF3:BF4"/>
+    <mergeCell ref="BG3:BG4"/>
+    <mergeCell ref="BH3:BH4"/>
+    <mergeCell ref="BA3:BA4"/>
+    <mergeCell ref="BB3:BB4"/>
+    <mergeCell ref="BC3:BC4"/>
+    <mergeCell ref="BD3:BD4"/>
+    <mergeCell ref="BE3:BE4"/>
+    <mergeCell ref="AV3:AV4"/>
+    <mergeCell ref="AW3:AW4"/>
+    <mergeCell ref="AX3:AX4"/>
+    <mergeCell ref="AY3:AY4"/>
+    <mergeCell ref="AZ3:AZ4"/>
+    <mergeCell ref="AQ3:AQ4"/>
+    <mergeCell ref="AR3:AR4"/>
+    <mergeCell ref="AS3:AS4"/>
+    <mergeCell ref="AT3:AT4"/>
+    <mergeCell ref="AU3:AU4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AN3:AN4"/>
+    <mergeCell ref="AO3:AO4"/>
+    <mergeCell ref="AP3:AP4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AA3:AA4"/>
+    <mergeCell ref="AB3:AB4"/>
+    <mergeCell ref="AC3:AC4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="X3:X4"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="BA2:BB2"/>
+    <mergeCell ref="BC2:BD2"/>
+    <mergeCell ref="BE2:BF2"/>
+    <mergeCell ref="BG2:BH2"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="AY2:AZ2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
     <mergeCell ref="B58:E58"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:H2"/>
@@ -18984,81 +19106,6 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B57:E57"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="BA2:BB2"/>
-    <mergeCell ref="BC2:BD2"/>
-    <mergeCell ref="BE2:BF2"/>
-    <mergeCell ref="BG2:BH2"/>
-    <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AW2:AX2"/>
-    <mergeCell ref="AY2:AZ2"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Y4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AA3:AA4"/>
-    <mergeCell ref="AB3:AB4"/>
-    <mergeCell ref="AC3:AC4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="AJ3:AJ4"/>
-    <mergeCell ref="AL3:AL4"/>
-    <mergeCell ref="AM3:AM4"/>
-    <mergeCell ref="AN3:AN4"/>
-    <mergeCell ref="AO3:AO4"/>
-    <mergeCell ref="AP3:AP4"/>
-    <mergeCell ref="AQ3:AQ4"/>
-    <mergeCell ref="AR3:AR4"/>
-    <mergeCell ref="AS3:AS4"/>
-    <mergeCell ref="AT3:AT4"/>
-    <mergeCell ref="AU3:AU4"/>
-    <mergeCell ref="AV3:AV4"/>
-    <mergeCell ref="AW3:AW4"/>
-    <mergeCell ref="AX3:AX4"/>
-    <mergeCell ref="AY3:AY4"/>
-    <mergeCell ref="AZ3:AZ4"/>
-    <mergeCell ref="BF3:BF4"/>
-    <mergeCell ref="BG3:BG4"/>
-    <mergeCell ref="BH3:BH4"/>
-    <mergeCell ref="BA3:BA4"/>
-    <mergeCell ref="BB3:BB4"/>
-    <mergeCell ref="BC3:BC4"/>
-    <mergeCell ref="BD3:BD4"/>
-    <mergeCell ref="BE3:BE4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -19073,7 +19120,7 @@
   </sheetPr>
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
@@ -19101,45 +19148,45 @@
     </row>
     <row r="2" spans="1:12" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="84" t="s">
         <v>312</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
       <c r="G2" s="2"/>
-      <c r="I2" s="97" t="s">
-        <v>929</v>
-      </c>
-      <c r="J2" s="98"/>
+      <c r="I2" s="100" t="s">
+        <v>928</v>
+      </c>
+      <c r="J2" s="101"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="106"/>
       <c r="G3" s="1"/>
-      <c r="I3" s="82" t="s">
+      <c r="I3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="J3" s="84" t="s">
+      <c r="J3" s="89" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="97" t="s">
         <v>313</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99"/>
       <c r="G4" s="1"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="95"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="103"/>
     </row>
     <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
@@ -19166,17 +19213,17 @@
         <v>37</v>
       </c>
       <c r="D6" s="42" t="s">
+        <v>929</v>
+      </c>
+      <c r="E6" s="43" t="s">
         <v>930</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>931</v>
       </c>
       <c r="G6" s="1"/>
       <c r="I6" s="41" t="s">
+        <v>943</v>
+      </c>
+      <c r="J6" s="41" t="s">
         <v>944</v>
-      </c>
-      <c r="J6" s="41" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
@@ -19188,17 +19235,17 @@
         <v>37</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="G7" s="1"/>
       <c r="I7" s="41" t="s">
+        <v>910</v>
+      </c>
+      <c r="J7" s="41" t="s">
         <v>911</v>
-      </c>
-      <c r="J7" s="41" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
@@ -19210,17 +19257,17 @@
         <v>37</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="G8" s="1"/>
       <c r="I8" s="41" t="s">
+        <v>912</v>
+      </c>
+      <c r="J8" s="41" t="s">
         <v>913</v>
-      </c>
-      <c r="J8" s="41" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
@@ -19232,17 +19279,17 @@
         <v>37</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="G9" s="1"/>
       <c r="I9" s="41" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="J9" s="41" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
@@ -19254,17 +19301,17 @@
         <v>37</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="G10" s="1"/>
       <c r="I10" s="41" t="s">
+        <v>916</v>
+      </c>
+      <c r="J10" s="41" t="s">
         <v>917</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
@@ -19276,17 +19323,17 @@
         <v>37</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="G11" s="1"/>
       <c r="I11" s="41" t="s">
+        <v>918</v>
+      </c>
+      <c r="J11" s="41" t="s">
         <v>919</v>
-      </c>
-      <c r="J11" s="41" t="s">
-        <v>920</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
@@ -19298,17 +19345,17 @@
         <v>37</v>
       </c>
       <c r="D12" s="42" t="s">
+        <v>941</v>
+      </c>
+      <c r="E12" s="43" t="s">
         <v>942</v>
-      </c>
-      <c r="E12" s="43" t="s">
-        <v>943</v>
       </c>
       <c r="G12" s="1"/>
       <c r="I12" s="41" t="s">
+        <v>920</v>
+      </c>
+      <c r="J12" s="41" t="s">
         <v>921</v>
-      </c>
-      <c r="J12" s="41" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.35">
@@ -19335,7 +19382,7 @@
       </c>
       <c r="G14" s="1"/>
       <c r="I14" s="76" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="J14" s="76"/>
       <c r="L14" s="78"/>
@@ -19356,7 +19403,7 @@
       </c>
       <c r="G15" s="1"/>
       <c r="I15" s="76" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="J15" s="76"/>
       <c r="L15" s="78"/>
@@ -19492,10 +19539,10 @@
       </c>
       <c r="G23" s="1"/>
       <c r="I23" s="55" t="s">
+        <v>931</v>
+      </c>
+      <c r="J23" s="55" t="s">
         <v>932</v>
-      </c>
-      <c r="J23" s="55" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
@@ -19650,10 +19697,10 @@
       </c>
       <c r="G33" s="1"/>
       <c r="I33" s="55" t="s">
+        <v>933</v>
+      </c>
+      <c r="J33" s="55" t="s">
         <v>934</v>
-      </c>
-      <c r="J33" s="55" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -19938,32 +19985,32 @@
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
-      <c r="B53" s="92" t="s">
+      <c r="B53" s="84" t="s">
         <v>312</v>
       </c>
-      <c r="C53" s="93"/>
-      <c r="D53" s="93"/>
-      <c r="E53" s="94"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="86"/>
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
-      <c r="B54" s="102" t="s">
+      <c r="B54" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="103"/>
-      <c r="D54" s="103"/>
-      <c r="E54" s="104"/>
+      <c r="C54" s="105"/>
+      <c r="D54" s="105"/>
+      <c r="E54" s="106"/>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
-      <c r="B55" s="99" t="s">
+      <c r="B55" s="97" t="s">
         <v>314</v>
       </c>
-      <c r="C55" s="100"/>
-      <c r="D55" s="100"/>
-      <c r="E55" s="101"/>
+      <c r="C55" s="98"/>
+      <c r="D55" s="98"/>
+      <c r="E55" s="99"/>
       <c r="G55" s="1"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -19996,10 +20043,10 @@
       <c r="E57" s="7"/>
       <c r="G57" s="1"/>
       <c r="I57" s="65" t="s">
+        <v>974</v>
+      </c>
+      <c r="J57" s="65" t="s">
         <v>975</v>
-      </c>
-      <c r="J57" s="65" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -20098,13 +20145,13 @@
       </c>
       <c r="G65" s="1"/>
       <c r="I65" s="67" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="J65" s="67" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="K65" s="65" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -20123,13 +20170,13 @@
       </c>
       <c r="G66" s="1"/>
       <c r="I66" s="67" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="J66" s="67" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="K66" s="65" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -20252,10 +20299,10 @@
       </c>
       <c r="G74" s="1"/>
       <c r="I74" s="44" t="s">
+        <v>945</v>
+      </c>
+      <c r="J74" s="44" t="s">
         <v>946</v>
-      </c>
-      <c r="J74" s="44" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -20274,10 +20321,10 @@
       </c>
       <c r="G75" s="1"/>
       <c r="I75" s="45" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="J75" s="45" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -20296,10 +20343,10 @@
       </c>
       <c r="G76" s="1"/>
       <c r="I76" s="45" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="J76" s="45" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -20318,10 +20365,10 @@
       </c>
       <c r="G77" s="1"/>
       <c r="I77" s="45" t="s">
+        <v>924</v>
+      </c>
+      <c r="J77" s="45" t="s">
         <v>925</v>
-      </c>
-      <c r="J77" s="45" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -20340,10 +20387,10 @@
       </c>
       <c r="G78" s="1"/>
       <c r="I78" s="77" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="J78" s="77" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -20362,10 +20409,10 @@
       </c>
       <c r="G79" s="1"/>
       <c r="I79" s="77" t="s">
+        <v>1015</v>
+      </c>
+      <c r="J79" s="77" t="s">
         <v>1016</v>
-      </c>
-      <c r="J79" s="77" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -20440,10 +20487,10 @@
       </c>
       <c r="G84" s="1"/>
       <c r="I84" s="76" t="s">
+        <v>1018</v>
+      </c>
+      <c r="J84" s="75" t="s">
         <v>1019</v>
-      </c>
-      <c r="J84" s="75" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -20461,11 +20508,11 @@
         <v>319</v>
       </c>
       <c r="G85" s="1"/>
-      <c r="I85" s="106" t="s">
+      <c r="I85" s="80" t="s">
+        <v>1028</v>
+      </c>
+      <c r="J85" s="79" t="s">
         <v>1029</v>
-      </c>
-      <c r="J85" s="105" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -20718,20 +20765,20 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}">
-      <selection activeCell="M58" sqref="M58"/>
+    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}">
+      <selection activeCell="I2" sqref="I2:J2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+      <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
     </customSheetView>
     <customSheetView guid="{0FB11559-FF5E-4B68-9C91-951C6118F018}" topLeftCell="A51">
       <selection activeCell="G87" sqref="G87"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}">
-      <selection activeCell="I2" sqref="I2:J2"/>
+    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}">
+      <selection activeCell="M58" sqref="M58"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="9">
@@ -20752,14 +20799,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20798,104 +20845,104 @@
     </row>
     <row r="2" spans="1:23" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="84" t="s">
         <v>376</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94"/>
-      <c r="G2" s="97" t="s">
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
+      <c r="G2" s="100" t="s">
         <v>820</v>
       </c>
-      <c r="H2" s="98"/>
-      <c r="J2" s="97" t="s">
+      <c r="H2" s="101"/>
+      <c r="J2" s="100" t="s">
         <v>821</v>
       </c>
-      <c r="K2" s="98"/>
-      <c r="M2" s="97" t="s">
+      <c r="K2" s="101"/>
+      <c r="M2" s="100" t="s">
         <v>821</v>
       </c>
-      <c r="N2" s="98"/>
-      <c r="P2" s="97" t="s">
+      <c r="N2" s="101"/>
+      <c r="P2" s="100" t="s">
         <v>880</v>
       </c>
-      <c r="Q2" s="98"/>
-      <c r="S2" s="97" t="s">
-        <v>888</v>
-      </c>
-      <c r="T2" s="98"/>
-      <c r="V2" s="97" t="s">
-        <v>888</v>
-      </c>
-      <c r="W2" s="98"/>
+      <c r="Q2" s="101"/>
+      <c r="S2" s="100" t="s">
+        <v>887</v>
+      </c>
+      <c r="T2" s="101"/>
+      <c r="V2" s="100" t="s">
+        <v>887</v>
+      </c>
+      <c r="W2" s="101"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
-      <c r="G3" s="82" t="s">
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="106"/>
+      <c r="G3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="J3" s="82" t="s">
+      <c r="J3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="K3" s="84" t="s">
+      <c r="K3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="M3" s="82" t="s">
+      <c r="M3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="N3" s="84" t="s">
+      <c r="N3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="P3" s="82" t="s">
+      <c r="P3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="Q3" s="84" t="s">
+      <c r="Q3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="S3" s="82" t="s">
+      <c r="S3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="T3" s="84" t="s">
+      <c r="T3" s="89" t="s">
         <v>302</v>
       </c>
-      <c r="V3" s="82" t="s">
+      <c r="V3" s="87" t="s">
         <v>301</v>
       </c>
-      <c r="W3" s="84" t="s">
+      <c r="W3" s="89" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="97" t="s">
         <v>377</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="95"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="95"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="95"/>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="95"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="95"/>
-      <c r="V4" s="96"/>
-      <c r="W4" s="95"/>
-    </row>
-    <row r="5" spans="1:23" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="103"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="103"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="103"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="103"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="103"/>
+      <c r="V4" s="102"/>
+      <c r="W4" s="103"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>378</v>
@@ -20928,10 +20975,10 @@
         <v>849</v>
       </c>
       <c r="P5" s="26" t="s">
-        <v>881</v>
+        <v>1030</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="S5" s="26" t="s">
         <v>822</v>
@@ -20979,10 +21026,10 @@
         <v>849</v>
       </c>
       <c r="P6" s="26" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="S6" s="26" t="s">
         <v>823</v>
@@ -21069,10 +21116,10 @@
         <v>849</v>
       </c>
       <c r="P8" s="75" t="s">
+        <v>1020</v>
+      </c>
+      <c r="Q8" s="75" t="s">
         <v>1021</v>
-      </c>
-      <c r="Q8" s="75" t="s">
-        <v>1022</v>
       </c>
       <c r="S8" s="26" t="s">
         <v>825</v>
@@ -21114,10 +21161,10 @@
         <v>849</v>
       </c>
       <c r="P9" s="75" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="Q9" s="75" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="S9" s="26" t="s">
         <v>826</v>
@@ -21159,10 +21206,10 @@
         <v>849</v>
       </c>
       <c r="P10" s="75" t="s">
+        <v>1023</v>
+      </c>
+      <c r="Q10" s="75" t="s">
         <v>1024</v>
-      </c>
-      <c r="Q10" s="75" t="s">
-        <v>1025</v>
       </c>
       <c r="S10" s="26" t="s">
         <v>827</v>
@@ -21525,30 +21572,30 @@
     </row>
     <row r="25" spans="1:20" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1"/>
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="84" t="s">
         <v>376</v>
       </c>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="94"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="86"/>
     </row>
     <row r="26" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="102" t="s">
+      <c r="B26" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="103"/>
-      <c r="D26" s="103"/>
-      <c r="E26" s="104"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="106"/>
     </row>
     <row r="27" spans="1:20" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1"/>
-      <c r="B27" s="99" t="s">
+      <c r="B27" s="97" t="s">
         <v>382</v>
       </c>
-      <c r="C27" s="100"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="101"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="99"/>
     </row>
     <row r="28" spans="1:20" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
@@ -21849,43 +21896,44 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}">
+      <selection activeCell="J25" sqref="J25:K41"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="V16" sqref="V16"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}">
-      <selection activeCell="J25" sqref="J25:K41"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="24">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="W3:W4"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21910,31 +21958,31 @@
   <sheetData>
     <row r="1" spans="2:13" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:13" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="84" t="s">
         <v>408</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
     </row>
     <row r="3" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="104" t="s">
         <v>409</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="104"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="106"/>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
       <c r="M3" s="26"/>
     </row>
     <row r="4" spans="2:13" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="97" t="s">
         <v>410</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99"/>
     </row>
     <row r="5" spans="2:13" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
@@ -23617,13 +23665,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" scale="70" topLeftCell="A58">
-      <selection activeCell="G11" sqref="G11"/>
+    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}" scale="70">
+      <selection activeCell="H4" sqref="H4:H14"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{E564F581-258D-40EE-A8FC-D3934E0E049F}" scale="70">
-      <selection activeCell="H4" sqref="H4:H14"/>
+    <customSheetView guid="{707DC1D0-2077-4C17-8276-287DF75CEF77}" scale="70" topLeftCell="A58">
+      <selection activeCell="G11" sqref="G11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
     </customSheetView>

</xml_diff>